<commit_message>
split PHSMs periods into two stage
</commit_message>
<xml_diff>
--- a/data/disease_class.xlsx
+++ b/data/disease_class.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kanggle-my.sharepoint.com/personal/phonedata_kanggle_onmicrosoft_com/Documents/XMU/likangguo/2022/11 COVID_impact_luoli/code_PHSM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_C38AD33000696FAAA8F4329D47BF08939259ED04" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33F69F93-C07B-499A-8508-6B9433C8FC0E}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_C38AD33000696FAAA8F4329D47BF08939259ED04" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90E4BC46-0B82-4561-896C-E99911435AA2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
   <si>
-    <t>class</t>
-  </si>
-  <si>
     <t>diseasename</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
   </si>
   <si>
     <t>流行性出血热</t>
-  </si>
-  <si>
-    <t>Japanese encephalitis</t>
   </si>
   <si>
     <t>乙型脑炎</t>
@@ -195,6 +189,14 @@
   </si>
   <si>
     <t>AHC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Japanese encephalitis</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -255,6 +257,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -539,367 +545,369 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
         <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
         <v>45</v>
-      </c>
-      <c r="B21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>